<commit_message>
no es mucho pero es trabajo honesto
</commit_message>
<xml_diff>
--- a/Codigos ENS.xlsx
+++ b/Codigos ENS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rarav\Dropbox\2022\CURSOS-1er\EYP2020\EYP3007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\home\Documents\cursos-UC\EYP-3007\consultoria-t1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB3166E9-D0B5-4DB5-A80B-16FDC0DC5106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF79E4A-813C-456F-B71A-0C9D143F60DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1078,7 +1078,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1097,6 +1097,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1261,7 +1267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1279,10 +1285,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1603,19 +1613,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54" style="1" customWidth="1"/>
-    <col min="4" max="4" width="69.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>312</v>
       </c>
@@ -1629,8 +1639,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>314</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1643,8 +1653,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1655,8 +1665,8 @@
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1667,8 +1677,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1679,8 +1689,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>328</v>
       </c>
@@ -1691,8 +1701,8 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1703,14 +1713,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="22"/>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>313</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1723,8 +1733,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1735,8 +1745,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1747,8 +1757,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1759,8 +1769,8 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1771,8 +1781,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1783,8 +1793,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1795,8 +1805,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1807,8 +1817,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>315</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1821,8 +1831,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="18"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1833,8 +1843,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1845,8 +1855,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1857,8 +1867,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="18"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1869,8 +1879,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1881,8 +1891,8 @@
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1893,8 +1903,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>316</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1907,8 +1917,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
       <c r="B25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1919,8 +1929,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
       <c r="B26" s="4" t="s">
         <v>24</v>
       </c>
@@ -1931,8 +1941,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
       <c r="B27" s="4" t="s">
         <v>25</v>
       </c>
@@ -1943,8 +1953,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
       <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
@@ -1955,8 +1965,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>317</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1969,8 +1979,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1981,8 +1991,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="18"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1993,8 +2003,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="18"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2005,32 +2015,32 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="17" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="17" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2041,8 +2051,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="18"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2053,8 +2063,8 @@
         <v>278</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2065,8 +2075,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="18"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2077,32 +2087,32 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="18"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="17" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="17" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
         <v>318</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -2115,8 +2125,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="17"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
       <c r="B42" s="4" t="s">
         <v>40</v>
       </c>
@@ -2127,8 +2137,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="17"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
       <c r="B43" s="4" t="s">
         <v>41</v>
       </c>
@@ -2139,8 +2149,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="17"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
       <c r="B44" s="4" t="s">
         <v>42</v>
       </c>
@@ -2151,8 +2161,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="17"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
       <c r="B45" s="4" t="s">
         <v>43</v>
       </c>
@@ -2163,8 +2173,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="17"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
       <c r="B46" s="4" t="s">
         <v>44</v>
       </c>
@@ -2175,8 +2185,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="17"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
       <c r="B47" s="4" t="s">
         <v>45</v>
       </c>
@@ -2187,8 +2197,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="17"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
       <c r="B48" s="4" t="s">
         <v>46</v>
       </c>
@@ -2199,8 +2209,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="17"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
         <v>47</v>
       </c>
@@ -2211,8 +2221,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="17"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
       <c r="B50" s="4" t="s">
         <v>48</v>
       </c>
@@ -2223,8 +2233,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="17"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
       <c r="B51" s="4" t="s">
         <v>49</v>
       </c>
@@ -2235,8 +2245,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="18" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
         <v>319</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2249,8 +2259,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="19"/>
       <c r="B53" s="2" t="s">
         <v>51</v>
       </c>
@@ -2261,8 +2271,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="18"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
       <c r="B54" s="2" t="s">
         <v>52</v>
       </c>
@@ -2273,8 +2283,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="18"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="19"/>
       <c r="B55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2285,8 +2295,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="18"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
@@ -2297,8 +2307,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="18"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
       <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2309,8 +2319,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="18"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
       <c r="B58" s="2" t="s">
         <v>56</v>
       </c>
@@ -2321,8 +2331,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="17" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
         <v>320</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -2335,8 +2345,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="17"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
       <c r="B60" s="4" t="s">
         <v>58</v>
       </c>
@@ -2347,8 +2357,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="17"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
       <c r="B61" s="4" t="s">
         <v>59</v>
       </c>
@@ -2359,8 +2369,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="17"/>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="18"/>
       <c r="B62" s="4" t="s">
         <v>60</v>
       </c>
@@ -2371,8 +2381,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="17"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
       <c r="B63" s="4" t="s">
         <v>61</v>
       </c>
@@ -2383,8 +2393,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="17"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
       <c r="B64" s="4" t="s">
         <v>62</v>
       </c>
@@ -2395,8 +2405,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="17"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
       <c r="B65" s="4" t="s">
         <v>63</v>
       </c>
@@ -2407,8 +2417,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="17"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
       <c r="B66" s="4" t="s">
         <v>64</v>
       </c>
@@ -2419,8 +2429,8 @@
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="17"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
       <c r="B67" s="4" t="s">
         <v>65</v>
       </c>
@@ -2431,8 +2441,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="18" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
         <v>321</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -2441,24 +2451,24 @@
       <c r="C68" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="18"/>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
       <c r="B69" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="18"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="20"/>
       <c r="B70" s="2" t="s">
         <v>68</v>
       </c>
@@ -2469,8 +2479,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="20"/>
       <c r="B71" s="2" t="s">
         <v>69</v>
       </c>
@@ -2481,44 +2491,44 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="18"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
       <c r="B72" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" s="18"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="20"/>
       <c r="B73" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="18"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="20"/>
       <c r="B74" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="18"/>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="20"/>
       <c r="B75" s="2" t="s">
         <v>73</v>
       </c>
@@ -2529,8 +2539,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="18"/>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="20"/>
       <c r="B76" s="2" t="s">
         <v>74</v>
       </c>
@@ -2541,32 +2551,32 @@
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="18"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="20"/>
       <c r="B77" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="17" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="18"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="20"/>
       <c r="B78" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="17" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
         <v>322</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2579,8 +2589,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" s="17"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="18"/>
       <c r="B80" s="4" t="s">
         <v>78</v>
       </c>
@@ -2591,8 +2601,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="17"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
       <c r="B81" s="4" t="s">
         <v>79</v>
       </c>
@@ -2603,8 +2613,8 @@
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="17"/>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="18"/>
       <c r="B82" s="4" t="s">
         <v>80</v>
       </c>
@@ -2615,8 +2625,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="17"/>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
       <c r="B83" s="4" t="s">
         <v>81</v>
       </c>
@@ -2627,8 +2637,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="18" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
         <v>323</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -2641,8 +2651,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" s="18"/>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="19"/>
       <c r="B85" s="2" t="s">
         <v>83</v>
       </c>
@@ -2653,8 +2663,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" s="18"/>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="19"/>
       <c r="B86" s="2" t="s">
         <v>84</v>
       </c>
@@ -2665,8 +2675,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" s="18"/>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="19"/>
       <c r="B87" s="2" t="s">
         <v>85</v>
       </c>
@@ -2677,8 +2687,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" s="18"/>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="19"/>
       <c r="B88" s="2" t="s">
         <v>86</v>
       </c>
@@ -2689,8 +2699,8 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" s="18"/>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="19"/>
       <c r="B89" s="2" t="s">
         <v>87</v>
       </c>
@@ -2701,8 +2711,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A90" s="18"/>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="19"/>
       <c r="B90" s="2" t="s">
         <v>88</v>
       </c>
@@ -2713,8 +2723,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" s="18"/>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="19"/>
       <c r="B91" s="2" t="s">
         <v>89</v>
       </c>
@@ -2725,8 +2735,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" s="17" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="18" t="s">
         <v>324</v>
       </c>
       <c r="B92" s="4" t="s">
@@ -2739,8 +2749,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" s="17"/>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="18"/>
       <c r="B93" s="4" t="s">
         <v>91</v>
       </c>
@@ -2751,8 +2761,8 @@
         <v>308</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" s="17"/>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="18"/>
       <c r="B94" s="4" t="s">
         <v>92</v>
       </c>
@@ -2763,8 +2773,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" s="17"/>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="18"/>
       <c r="B95" s="4" t="s">
         <v>93</v>
       </c>
@@ -2775,8 +2785,8 @@
         <v>309</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="17"/>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="18"/>
       <c r="B96" s="4" t="s">
         <v>94</v>
       </c>
@@ -2787,8 +2797,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="17"/>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="18"/>
       <c r="B97" s="4" t="s">
         <v>95</v>
       </c>
@@ -2799,8 +2809,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" s="17"/>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="18"/>
       <c r="B98" s="4" t="s">
         <v>96</v>
       </c>
@@ -2811,8 +2821,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" s="17"/>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="18"/>
       <c r="B99" s="4" t="s">
         <v>97</v>
       </c>
@@ -2823,8 +2833,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" s="17"/>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="18"/>
       <c r="B100" s="4" t="s">
         <v>98</v>
       </c>
@@ -2835,8 +2845,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" s="17"/>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="18"/>
       <c r="B101" s="4" t="s">
         <v>99</v>
       </c>
@@ -2847,8 +2857,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" s="17"/>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="18"/>
       <c r="B102" s="4" t="s">
         <v>100</v>
       </c>
@@ -2859,8 +2869,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A103" s="17"/>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="18"/>
       <c r="B103" s="4" t="s">
         <v>101</v>
       </c>
@@ -2871,8 +2881,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" s="18" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
@@ -2885,8 +2895,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" s="18"/>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="19"/>
       <c r="B105" s="2" t="s">
         <v>103</v>
       </c>
@@ -2897,8 +2907,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" s="18"/>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="19"/>
       <c r="B106" s="2" t="s">
         <v>104</v>
       </c>
@@ -2909,8 +2919,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" s="18"/>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="19"/>
       <c r="B107" s="2" t="s">
         <v>105</v>
       </c>
@@ -2921,8 +2931,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" s="18"/>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="19"/>
       <c r="B108" s="2" t="s">
         <v>106</v>
       </c>
@@ -2933,8 +2943,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" s="18"/>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="19"/>
       <c r="B109" s="2" t="s">
         <v>107</v>
       </c>
@@ -2945,8 +2955,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" s="18"/>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="19"/>
       <c r="B110" s="2" t="s">
         <v>108</v>
       </c>
@@ -2957,8 +2967,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A111" s="17" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="18" t="s">
         <v>325</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -2971,8 +2981,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A112" s="17"/>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="18"/>
       <c r="B112" s="4" t="s">
         <v>110</v>
       </c>
@@ -2983,8 +2993,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A113" s="17"/>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="18"/>
       <c r="B113" s="4" t="s">
         <v>111</v>
       </c>
@@ -2995,8 +3005,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A114" s="17"/>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="18"/>
       <c r="B114" s="4" t="s">
         <v>112</v>
       </c>
@@ -3007,8 +3017,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A115" s="17"/>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="18"/>
       <c r="B115" s="4" t="s">
         <v>113</v>
       </c>
@@ -3019,8 +3029,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A116" s="17"/>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="18"/>
       <c r="B116" s="4" t="s">
         <v>114</v>
       </c>
@@ -3031,8 +3041,8 @@
         <v>248</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A117" s="17"/>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="18"/>
       <c r="B117" s="4" t="s">
         <v>115</v>
       </c>
@@ -3043,8 +3053,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A118" s="17"/>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="18"/>
       <c r="B118" s="4" t="s">
         <v>116</v>
       </c>
@@ -3055,8 +3065,8 @@
         <v>250</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A119" s="17"/>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="18"/>
       <c r="B119" s="4" t="s">
         <v>117</v>
       </c>
@@ -3067,8 +3077,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A120" s="17"/>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="18"/>
       <c r="B120" s="4" t="s">
         <v>118</v>
       </c>
@@ -3079,8 +3089,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" s="17"/>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="18"/>
       <c r="B121" s="4" t="s">
         <v>119</v>
       </c>
@@ -3091,8 +3101,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A122" s="17"/>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="18"/>
       <c r="B122" s="4" t="s">
         <v>120</v>
       </c>
@@ -3103,8 +3113,8 @@
         <v>254</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123" s="17"/>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="18"/>
       <c r="B123" s="4" t="s">
         <v>121</v>
       </c>
@@ -3115,8 +3125,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A124" s="17"/>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="18"/>
       <c r="B124" s="4" t="s">
         <v>122</v>
       </c>
@@ -3127,8 +3137,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A125" s="17"/>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="18"/>
       <c r="B125" s="4" t="s">
         <v>123</v>
       </c>
@@ -3139,8 +3149,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A126" s="18" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="19" t="s">
         <v>326</v>
       </c>
       <c r="B126" s="2" t="s">
@@ -3153,8 +3163,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127" s="18"/>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="19"/>
       <c r="B127" s="2" t="s">
         <v>125</v>
       </c>
@@ -3165,8 +3175,8 @@
         <v>259</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A128" s="18"/>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="19"/>
       <c r="B128" s="2" t="s">
         <v>126</v>
       </c>
@@ -3177,8 +3187,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A129" s="18"/>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="19"/>
       <c r="B129" s="2" t="s">
         <v>127</v>
       </c>
@@ -3189,8 +3199,8 @@
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A130" s="18"/>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="19"/>
       <c r="B130" s="2" t="s">
         <v>128</v>
       </c>
@@ -3201,8 +3211,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A131" s="18"/>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="19"/>
       <c r="B131" s="2" t="s">
         <v>129</v>
       </c>
@@ -3213,8 +3223,8 @@
         <v>263</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A132" s="18"/>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="19"/>
       <c r="B132" s="2" t="s">
         <v>130</v>
       </c>
@@ -3225,8 +3235,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A133" s="18"/>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="19"/>
       <c r="B133" s="2" t="s">
         <v>131</v>
       </c>
@@ -3237,8 +3247,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A134" s="18"/>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="19"/>
       <c r="B134" s="2" t="s">
         <v>132</v>
       </c>
@@ -3249,8 +3259,8 @@
         <v>266</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A135" s="18"/>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="19"/>
       <c r="B135" s="2" t="s">
         <v>133</v>
       </c>
@@ -3261,8 +3271,8 @@
         <v>267</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A136" s="18"/>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="19"/>
       <c r="B136" s="2" t="s">
         <v>134</v>
       </c>
@@ -3273,8 +3283,8 @@
         <v>268</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A137" s="18"/>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="19"/>
       <c r="B137" s="2" t="s">
         <v>135</v>
       </c>
@@ -3285,8 +3295,8 @@
         <v>269</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A138" s="17" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="18" t="s">
         <v>327</v>
       </c>
       <c r="B138" s="4" t="s">
@@ -3299,8 +3309,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A139" s="17"/>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="18"/>
       <c r="B139" s="4" t="s">
         <v>137</v>
       </c>
@@ -3311,8 +3321,8 @@
         <v>271</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A140" s="17"/>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="18"/>
       <c r="B140" s="4" t="s">
         <v>138</v>
       </c>
@@ -3323,8 +3333,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A141" s="17"/>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="18"/>
       <c r="B141" s="4" t="s">
         <v>139</v>
       </c>
@@ -3335,8 +3345,8 @@
         <v>273</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A142" s="17"/>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="18"/>
       <c r="B142" s="4" t="s">
         <v>140</v>
       </c>
@@ -3347,8 +3357,8 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A143" s="17"/>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="18"/>
       <c r="B143" s="4" t="s">
         <v>141</v>
       </c>
@@ -3359,8 +3369,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A144" s="17"/>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="18"/>
       <c r="B144" s="4" t="s">
         <v>142</v>
       </c>

</xml_diff>